<commit_message>
configs/configure_dataset.py currently functions using the 'set' channel (functions the same as the 'pre' channel, just renamed); consider a future refactor (when actually needed) where a dataclass/dict holds default values that can be overridden from the CLI)
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -5159,13 +5159,13 @@
   </sheetPr>
   <dimension ref="A1:O654"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A637" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D663" activeCellId="0" sqref="D663"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A633" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F663" activeCellId="0" sqref="F663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Re-run experiments/2025-09-05 since previous run had spectral norm loss with lambda 1e-8
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -461,262 +461,262 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>2025-09-04 16:09:19</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>0000-00-00/a/0000</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
+      <c r="D2" s="4" t="inlineStr"/>
+      <c r="E2" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>[[1, 0], [1, 1]]</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="4" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4]</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>[0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224]</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="4" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4]</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" s="4" t="inlineStr">
         <is>
           <t>[0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224]</t>
         </is>
       </c>
-      <c r="M2" t="n">
+      <c r="M2" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2" s="4" t="n">
         <v>500</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2" s="4" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>2025-09-05 11:06:37</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>2025-09-05/a/0000</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
+      <c r="D3" s="4" t="inlineStr"/>
+      <c r="E3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr">
         <is>
           <t>[[1, 0], [1, 1]]</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="4" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="4" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19]</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="4" t="inlineStr">
         <is>
           <t>[0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806]</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" s="4" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9]</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L3" s="4" t="inlineStr">
         <is>
           <t>[0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612]</t>
         </is>
       </c>
-      <c r="M3" t="n">
+      <c r="M3" s="4" t="n">
         <v>5000</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3" s="4" t="n">
         <v>2500</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O3" s="4" t="n">
         <v>2500</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>2025-09-05 14:00:39</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t>2025-09-05/o/0000</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
+      <c r="D4" s="4" t="inlineStr"/>
+      <c r="E4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="4" t="inlineStr">
         <is>
           <t>[[1, 0], [1, 1]]</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="4" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="4" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" s="4" t="inlineStr">
         <is>
           <t>[1, 3, 5, 7, 9, 11, 13, 15, 17, 19]</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="4" t="inlineStr">
         <is>
           <t>[0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612]</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K4" s="4" t="inlineStr">
         <is>
           <t>[1, 3, 5, 7, 9]</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L4" s="4" t="inlineStr">
         <is>
           <t>[0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224]</t>
         </is>
       </c>
-      <c r="M4" t="n">
+      <c r="M4" s="4" t="n">
         <v>5000</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N4" s="4" t="n">
         <v>2500</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O4" s="4" t="n">
         <v>2500</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>2025-09-05 14:01:02</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="4" t="inlineStr">
         <is>
           <t>2025-09-05/e/0000</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="n">
+      <c r="D5" s="4" t="inlineStr"/>
+      <c r="E5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="4" t="inlineStr">
         <is>
           <t>[[1, 0], [1, 1]]</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="4" t="inlineStr">
         <is>
           <t>[0, 2, 4, 6, 8, 10, 12, 14, 16, 18, 20]</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" s="4" t="inlineStr">
         <is>
           <t>[0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294]</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="K5" s="4" t="inlineStr">
         <is>
           <t>[0, 2, 4, 6, 8, 10]</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L5" s="4" t="inlineStr">
         <is>
           <t>[0.1666666716337204, 0.1666666716337204, 0.1666666716337204, 0.1666666716337204, 0.1666666716337204, 0.1666666716337204]</t>
         </is>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" s="4" t="n">
         <v>5000</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N5" s="4" t="n">
         <v>2500</v>
       </c>
-      <c r="O5" t="n">
+      <c r="O5" s="4" t="n">
         <v>2500</v>
       </c>
     </row>
@@ -1115,1181 +1115,1252 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
-  <cols>
-    <col width="30.88" customWidth="1" style="4" min="1" max="1"/>
-    <col width="38.36" customWidth="1" style="4" min="3" max="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="5">
-      <c r="A1" s="6" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>timestamp</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>config_kind</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>config_id</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>loss_terms</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>loss_weights</t>
         </is>
       </c>
-      <c r="G1" s="6" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>optimizers</t>
         </is>
       </c>
-      <c r="H1" s="6" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>learning_rates</t>
         </is>
       </c>
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>train_batch_size</t>
         </is>
       </c>
-      <c r="J1" s="6" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>val_batch_size</t>
         </is>
       </c>
-      <c r="K1" s="6" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>early_stopping_strategy</t>
         </is>
       </c>
-      <c r="L1" s="6" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>early_stopping_patience</t>
         </is>
       </c>
-      <c r="M1" s="6" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>early_stopping_tol</t>
         </is>
       </c>
-      <c r="N1" s="6" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>num_epochs</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="5">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:18</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0000</t>
         </is>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>[1.0, 1e-08]</t>
         </is>
       </c>
-      <c r="G2" s="4" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H2" s="4" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I2" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J2" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K2" s="4" t="inlineStr">
+      <c r="I2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="L2" t="n">
         <v>8</v>
       </c>
-      <c r="M2" s="4" t="n">
+      <c r="M2" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N2" s="4" t="n">
+      <c r="N2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="5">
-      <c r="A3" s="4" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:21</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0001</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F3" s="4" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>[1.0, 3.162277660168379e-08]</t>
         </is>
       </c>
-      <c r="G3" s="4" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H3" s="4" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I3" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J3" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K3" s="4" t="inlineStr">
+      <c r="I3" t="n">
+        <v>128</v>
+      </c>
+      <c r="J3" t="n">
+        <v>128</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L3" s="4" t="n">
+      <c r="L3" t="n">
         <v>8</v>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="M3" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N3" s="4" t="n">
+      <c r="N3" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="5">
-      <c r="A4" s="4" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:23</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0002</t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F4" s="4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>[1.0, 1e-07]</t>
         </is>
       </c>
-      <c r="G4" s="4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H4" s="4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I4" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J4" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K4" s="4" t="inlineStr">
+      <c r="I4" t="n">
+        <v>128</v>
+      </c>
+      <c r="J4" t="n">
+        <v>128</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="L4" t="n">
         <v>8</v>
       </c>
-      <c r="M4" s="4" t="n">
+      <c r="M4" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N4" s="4" t="n">
+      <c r="N4" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" s="5">
-      <c r="A5" s="4" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:25</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0003</t>
         </is>
       </c>
-      <c r="E5" s="4" t="inlineStr">
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F5" s="4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>[1.0, 3.162277660168379e-07]</t>
         </is>
       </c>
-      <c r="G5" s="4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H5" s="4" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I5" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J5" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K5" s="4" t="inlineStr">
+      <c r="I5" t="n">
+        <v>128</v>
+      </c>
+      <c r="J5" t="n">
+        <v>128</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="L5" t="n">
         <v>8</v>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="M5" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N5" s="4" t="n">
+      <c r="N5" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" s="5">
-      <c r="A6" s="4" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:27</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0004</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F6" s="4" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>[1.0, 1e-06]</t>
         </is>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I6" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J6" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K6" s="4" t="inlineStr">
+      <c r="I6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L6" s="4" t="n">
+      <c r="L6" t="n">
         <v>8</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N6" s="4" t="n">
+      <c r="N6" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" s="5">
-      <c r="A7" s="4" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:30</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0005</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr">
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F7" s="4" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>[1.0, 3.162277660168379e-06]</t>
         </is>
       </c>
-      <c r="G7" s="4" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H7" s="4" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I7" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J7" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K7" s="4" t="inlineStr">
+      <c r="I7" t="n">
+        <v>128</v>
+      </c>
+      <c r="J7" t="n">
+        <v>128</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L7" s="4" t="n">
+      <c r="L7" t="n">
         <v>8</v>
       </c>
-      <c r="M7" s="4" t="n">
+      <c r="M7" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N7" s="4" t="n">
+      <c r="N7" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="5">
-      <c r="A8" s="4" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:32</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0006</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F8" s="4" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>[1.0, 1e-05]</t>
         </is>
       </c>
-      <c r="G8" s="4" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H8" s="4" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I8" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J8" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K8" s="4" t="inlineStr">
+      <c r="I8" t="n">
+        <v>128</v>
+      </c>
+      <c r="J8" t="n">
+        <v>128</v>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L8" s="4" t="n">
+      <c r="L8" t="n">
         <v>8</v>
       </c>
-      <c r="M8" s="4" t="n">
+      <c r="M8" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N8" s="4" t="n">
+      <c r="N8" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" s="5">
-      <c r="A9" s="4" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:34</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0007</t>
         </is>
       </c>
-      <c r="E9" s="4" t="inlineStr">
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F9" s="4" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>[1.0, 3.1622776601683795e-05]</t>
         </is>
       </c>
-      <c r="G9" s="4" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H9" s="4" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I9" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J9" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K9" s="4" t="inlineStr">
+      <c r="I9" t="n">
+        <v>128</v>
+      </c>
+      <c r="J9" t="n">
+        <v>128</v>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L9" s="4" t="n">
+      <c r="L9" t="n">
         <v>8</v>
       </c>
-      <c r="M9" s="4" t="n">
+      <c r="M9" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N9" s="4" t="n">
+      <c r="N9" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" s="5">
-      <c r="A10" s="4" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:37</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0008</t>
         </is>
       </c>
-      <c r="E10" s="4" t="inlineStr">
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F10" s="4" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>[1.0, 0.0001]</t>
         </is>
       </c>
-      <c r="G10" s="4" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H10" s="4" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I10" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J10" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K10" s="4" t="inlineStr">
+      <c r="I10" t="n">
+        <v>128</v>
+      </c>
+      <c r="J10" t="n">
+        <v>128</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L10" s="4" t="n">
+      <c r="L10" t="n">
         <v>8</v>
       </c>
-      <c r="M10" s="4" t="n">
+      <c r="M10" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N10" s="4" t="n">
+      <c r="N10" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1" s="5">
-      <c r="A11" s="4" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:39</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0009</t>
         </is>
       </c>
-      <c r="E11" s="4" t="inlineStr">
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F11" s="4" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>[1.0, 0.00031622776601683794]</t>
         </is>
       </c>
-      <c r="G11" s="4" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H11" s="4" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I11" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J11" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K11" s="4" t="inlineStr">
+      <c r="I11" t="n">
+        <v>128</v>
+      </c>
+      <c r="J11" t="n">
+        <v>128</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L11" s="4" t="n">
+      <c r="L11" t="n">
         <v>8</v>
       </c>
-      <c r="M11" s="4" t="n">
+      <c r="M11" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N11" s="4" t="n">
+      <c r="N11" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" s="5">
-      <c r="A12" s="4" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:41</t>
         </is>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C12" s="4" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0010</t>
         </is>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F12" s="4" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>[1.0, 0.001]</t>
         </is>
       </c>
-      <c r="G12" s="4" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H12" s="4" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I12" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J12" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K12" s="4" t="inlineStr">
+      <c r="I12" t="n">
+        <v>128</v>
+      </c>
+      <c r="J12" t="n">
+        <v>128</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L12" s="4" t="n">
+      <c r="L12" t="n">
         <v>8</v>
       </c>
-      <c r="M12" s="4" t="n">
+      <c r="M12" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N12" s="4" t="n">
+      <c r="N12" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" s="5">
-      <c r="A13" s="4" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:43</t>
         </is>
       </c>
-      <c r="B13" s="4" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C13" s="4" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0011</t>
         </is>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F13" s="4" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>[1.0, 0.0031622776601683794]</t>
         </is>
       </c>
-      <c r="G13" s="4" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H13" s="4" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I13" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J13" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K13" s="4" t="inlineStr">
+      <c r="I13" t="n">
+        <v>128</v>
+      </c>
+      <c r="J13" t="n">
+        <v>128</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L13" s="4" t="n">
+      <c r="L13" t="n">
         <v>8</v>
       </c>
-      <c r="M13" s="4" t="n">
+      <c r="M13" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N13" s="4" t="n">
+      <c r="N13" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" s="5">
-      <c r="A14" s="4" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:46</t>
         </is>
       </c>
-      <c r="B14" s="4" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C14" s="4" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0012</t>
         </is>
       </c>
-      <c r="E14" s="4" t="inlineStr">
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F14" s="4" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>[1.0, 0.01]</t>
         </is>
       </c>
-      <c r="G14" s="4" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H14" s="4" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I14" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J14" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K14" s="4" t="inlineStr">
+      <c r="I14" t="n">
+        <v>128</v>
+      </c>
+      <c r="J14" t="n">
+        <v>128</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L14" s="4" t="n">
+      <c r="L14" t="n">
         <v>8</v>
       </c>
-      <c r="M14" s="4" t="n">
+      <c r="M14" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N14" s="4" t="n">
+      <c r="N14" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" s="5">
-      <c r="A15" s="4" t="inlineStr">
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:48</t>
         </is>
       </c>
-      <c r="B15" s="4" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C15" s="4" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0013</t>
         </is>
       </c>
-      <c r="E15" s="4" t="inlineStr">
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F15" s="4" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>[1.0, 0.03162277660168379]</t>
         </is>
       </c>
-      <c r="G15" s="4" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H15" s="4" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I15" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J15" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K15" s="4" t="inlineStr">
+      <c r="I15" t="n">
+        <v>128</v>
+      </c>
+      <c r="J15" t="n">
+        <v>128</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L15" s="4" t="n">
+      <c r="L15" t="n">
         <v>8</v>
       </c>
-      <c r="M15" s="4" t="n">
+      <c r="M15" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N15" s="4" t="n">
+      <c r="N15" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1" s="5">
-      <c r="A16" s="4" t="inlineStr">
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:50</t>
         </is>
       </c>
-      <c r="B16" s="4" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C16" s="4" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0014</t>
         </is>
       </c>
-      <c r="E16" s="4" t="inlineStr">
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F16" s="4" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>[1.0, 0.1]</t>
         </is>
       </c>
-      <c r="G16" s="4" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H16" s="4" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I16" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J16" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K16" s="4" t="inlineStr">
+      <c r="I16" t="n">
+        <v>128</v>
+      </c>
+      <c r="J16" t="n">
+        <v>128</v>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L16" s="4" t="n">
+      <c r="L16" t="n">
         <v>8</v>
       </c>
-      <c r="M16" s="4" t="n">
+      <c r="M16" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N16" s="4" t="n">
+      <c r="N16" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" s="5">
-      <c r="A17" s="4" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:53</t>
         </is>
       </c>
-      <c r="B17" s="4" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C17" s="4" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0015</t>
         </is>
       </c>
-      <c r="E17" s="4" t="inlineStr">
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F17" s="4" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>[1.0, 0.31622776601683794]</t>
         </is>
       </c>
-      <c r="G17" s="4" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H17" s="4" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I17" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J17" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K17" s="4" t="inlineStr">
+      <c r="I17" t="n">
+        <v>128</v>
+      </c>
+      <c r="J17" t="n">
+        <v>128</v>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L17" s="4" t="n">
+      <c r="L17" t="n">
         <v>8</v>
       </c>
-      <c r="M17" s="4" t="n">
+      <c r="M17" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N17" s="4" t="n">
+      <c r="N17" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1" s="5">
-      <c r="A18" s="4" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:55</t>
         </is>
       </c>
-      <c r="B18" s="4" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C18" s="4" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0016</t>
         </is>
       </c>
-      <c r="E18" s="4" t="inlineStr">
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F18" s="4" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>[1.0, 1.0]</t>
         </is>
       </c>
-      <c r="G18" s="4" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H18" s="4" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I18" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J18" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K18" s="4" t="inlineStr">
+      <c r="I18" t="n">
+        <v>128</v>
+      </c>
+      <c r="J18" t="n">
+        <v>128</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L18" s="4" t="n">
+      <c r="L18" t="n">
         <v>8</v>
       </c>
-      <c r="M18" s="4" t="n">
+      <c r="M18" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N18" s="4" t="n">
+      <c r="N18" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="19" ht="15" customHeight="1" s="5">
-      <c r="A19" s="4" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>2025-09-05 11:27:30</t>
         </is>
       </c>
-      <c r="B19" s="4" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C19" s="4" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>configs/training/0000-00-00/b/0000</t>
         </is>
       </c>
-      <c r="E19" s="4" t="inlineStr">
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F19" s="4" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>[1.0, 1.0]</t>
         </is>
       </c>
-      <c r="G19" s="4" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H19" s="4" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I19" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J19" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K19" s="4" t="inlineStr">
+      <c r="I19" t="n">
+        <v>128</v>
+      </c>
+      <c r="J19" t="n">
+        <v>128</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L19" s="4" t="n">
+      <c r="L19" t="n">
         <v>8</v>
       </c>
-      <c r="M19" s="4" t="n">
+      <c r="M19" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N19" s="4" t="n">
+      <c r="N19" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1" s="5">
-      <c r="A20" s="4" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="inlineStr">
         <is>
           <t>2025-09-05 11:36:59</t>
         </is>
       </c>
-      <c r="B20" s="4" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C20" s="4" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>configs/training/0000-00-00/a/0000</t>
         </is>
       </c>
-      <c r="E20" s="4" t="inlineStr">
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
         <is>
           <t>['cross_entropy']</t>
         </is>
       </c>
-      <c r="F20" s="4" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>[1.0]</t>
         </is>
       </c>
-      <c r="G20" s="4" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H20" s="4" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>[0.001]</t>
         </is>
       </c>
-      <c r="I20" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J20" s="4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K20" s="4" t="inlineStr">
+      <c r="I20" t="n">
+        <v>128</v>
+      </c>
+      <c r="J20" t="n">
+        <v>128</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L20" s="4" t="n">
+      <c r="L20" t="n">
         <v>8</v>
       </c>
-      <c r="M20" s="4" t="n">
+      <c r="M20" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N20" s="4" t="n">
+      <c r="N20" t="n">
         <v>500</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-09-05 15:27:52</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>configs/training/2025-09-05/a/0001</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['cross_entropy']</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>[1.0]</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>['torch.optim.adamw.AdamW']</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>[0.001]</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>128</v>
+      </c>
+      <c r="J21" t="n">
+        <v>128</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>general_utils.ml.training.NoImprovementStopping</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>8</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="N21" t="n">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Revert "Revert to 67dbc07"
This reverts commit 93a29170d9c84908c8eec312f92a6d30c8716b6a.
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="161">
   <si>
     <t xml:space="preserve">timestamp</t>
   </si>
@@ -175,64 +175,79 @@
     <t xml:space="preserve">readout_network_dropouts</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-08-15 14:19:10</t>
+    <t xml:space="preserve">2025-09-09 11:08:49</t>
   </si>
   <si>
     <t xml:space="preserve">models</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-08-15/a/0000</t>
-  </si>
-  <si>
     <t xml:space="preserve">models.networks.FCN</t>
   </si>
   <si>
+    <t xml:space="preserve">['embedding_dim___', 10]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
   </si>
   <si>
     <t xml:space="preserve">[None]</t>
   </si>
   <si>
+    <t xml:space="preserve">torch.nn.modules.rnn.RNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tanh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[20, 20, 2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.5, None]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-09-09 11:09:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-00-00/b/0000</t>
+  </si>
+  <si>
     <t xml:space="preserve">torch.nn.modules.rnn.GRU</t>
   </si>
   <si>
+    <t xml:space="preserve">2025-09-09 11:12:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-09-09/b/0000</t>
+  </si>
+  <si>
     <t xml:space="preserve">embedding_dim___</t>
   </si>
   <si>
-    <t xml:space="preserve">[20, 20, 2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.5, None]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-08-19 10:30:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-08-19/a/0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-09-05 11:15:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-00-00/b/0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['embedding_dim___', 10]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">torch.nn.modules.rnn.RNN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tanh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-09-05 11:16:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-09-05/b/0000</t>
+    <t xml:space="preserve">2025-09-09 11:12:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-09-09/a/0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-09-09 11:12:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-09-09/a/0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[100, 20, 2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-09-09 11:13:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-09-09/a/0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1000, 20, 2]</t>
   </si>
   <si>
     <t xml:space="preserve">loss_terms</t>
@@ -793,7 +808,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,7 +855,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -885,7 +900,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -930,7 +945,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -975,7 +990,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -1036,18 +1051,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1097,185 +1112,267 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="M2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K3" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="M3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O3" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P3" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="C4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H4" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J5" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L5" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="M5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O5" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P5" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="C6" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H6" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="K6" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P6" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="C7" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K7" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L7" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="O5" s="2" t="s">
+      <c r="M7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P7" s="0" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1303,10 +1400,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="24.02"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1320,894 +1417,894 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="E2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L3" s="0" t="n">
+      <c r="C4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M4" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N4" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="I5" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="L5" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L4" s="0" t="n">
+      <c r="C6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L6" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M6" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N6" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="0" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L5" s="0" t="n">
+      <c r="C7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L7" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M7" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N7" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H6" s="0" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L6" s="0" t="n">
+      <c r="C8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M8" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N8" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="0" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L7" s="0" t="n">
+      <c r="C9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M9" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N9" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="0" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L8" s="0" t="n">
+      <c r="C10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M10" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N10" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" s="0" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L9" s="0" t="n">
+      <c r="C11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M11" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N11" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" s="0" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I10" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L10" s="0" t="n">
+      <c r="C12" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L12" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M12" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N12" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="0" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L11" s="0" t="n">
+      <c r="C13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M13" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N13" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="0" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L12" s="0" t="n">
+      <c r="C14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M14" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N14" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="0" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L13" s="0" t="n">
+      <c r="C15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M15" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N15" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="0" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I14" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L14" s="0" t="n">
+      <c r="C16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L16" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M16" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N16" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="0" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L15" s="0" t="n">
+      <c r="C17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L17" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M17" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N17" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="0" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I16" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L16" s="0" t="n">
+      <c r="C18" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M18" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N18" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" s="0" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L17" s="0" t="n">
+      <c r="C19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M19" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="N19" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H18" s="0" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I18" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L18" s="0" t="n">
+      <c r="C20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="M20" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="N20" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="0" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I19" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L19" s="0" t="n">
+      <c r="C21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="M21" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="N21" s="2" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L20" s="0" t="n">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L22" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M22" s="2" t="n">
         <v>1E-005</v>
       </c>
-      <c r="N20" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="M21" s="0" t="n">
-        <v>1E-005</v>
-      </c>
-      <c r="N21" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="L22" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="M22" s="0" t="n">
-        <v>1E-005</v>
-      </c>
-      <c r="N22" s="0" t="n">
+      <c r="N22" s="2" t="n">
         <v>500</v>
       </c>
     </row>
@@ -2229,7 +2326,7 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2252,53 +2349,53 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Previous commit missed configs/logs.xlsx
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" state="visible" r:id="rId3"/>
@@ -595,16 +595,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1053,13 +1057,13 @@
   </sheetPr>
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,266 +1117,266 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P4" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="L5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="N5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="O5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="0" t="s">
+      <c r="P5" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="L6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="N6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="O6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="P6" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="3" t="n">
         <v>1000</v>
       </c>
-      <c r="L7" s="0" t="s">
+      <c r="L7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M7" s="0" t="s">
+      <c r="M7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="0" t="s">
+      <c r="N7" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O7" s="0" t="s">
+      <c r="O7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="0" t="s">
+      <c r="P7" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2326,8 +2330,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Generate training config 2025-09-16/z/0000 with just cross entropy loss, prepare for running experiments/2025-09-16/0001
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -1258,7 +1258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2611,6 +2611,64 @@
         <v>1e-05</v>
       </c>
       <c r="N23" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:29:08</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>configs/training/2025-09-16/z/0000</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>['cross_entropy']</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>[1.0]</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>['torch.optim.adam.Adam']</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>[0.001]</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>128</v>
+      </c>
+      <c r="J24" t="n">
+        <v>128</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>general_utils.ml.training.NoImprovementStopping</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>8</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="N24" t="n">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit in advance of running experiment 2025-09-16/0002
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -1258,7 +1258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2669,6 +2669,64 @@
         <v>1e-05</v>
       </c>
       <c r="N24" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-09-16 14:13:04</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>configs/training/2025-09-16/x/0000</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>['cross_entropy', 'spectral_entropy']</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>[1.0, 0.01]</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>['torch.optim.adamw.AdamW', 'torch.optim.adam.Adam']</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>[0.001, 0.001]</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>128</v>
+      </c>
+      <c r="J25" t="n">
+        <v>128</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>general_utils.ml.training.NoImprovementStopping</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>8</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="N25" t="n">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit in advance of running experiment 2025-09-16/0003
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -1258,7 +1258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2727,6 +2727,64 @@
         <v>1e-05</v>
       </c>
       <c r="N25" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-09-16 14:27:00</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>training</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>configs/training/2025-09-16/x/0001</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>['cross_entropy', 'spectral_entropy']</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>[1.0, 0.01]</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>['torch.optim.adamw.AdamW', 'torch.optim.adam.Adam']</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>[0.001, 0.001]</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>128</v>
+      </c>
+      <c r="J26" t="n">
+        <v>128</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>general_utils.ml.training.NoImprovementStopping</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>20</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="N26" t="n">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prepare for experiment 2025-10-14/0000
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -732,523 +732,598 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
-  <cols>
-    <col width="31" customWidth="1" style="6" min="1" max="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>timestamp</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>config_kind</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>config_id</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>input_network</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="7" t="inlineStr">
         <is>
           <t>input_network_layer_sizes</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="7" t="inlineStr">
         <is>
           <t>input_network_nonlinearities</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="7" t="inlineStr">
         <is>
           <t>input_network_dropouts</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="7" t="inlineStr">
         <is>
           <t>rnn_type</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="7" t="inlineStr">
         <is>
           <t>rnn_input_size</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="7" t="inlineStr">
         <is>
           <t>rnn_hidden_size</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="7" t="inlineStr">
         <is>
           <t>rnn_nonlinearity</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="M1" s="7" t="inlineStr">
         <is>
           <t>readout_network</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="N1" s="7" t="inlineStr">
         <is>
           <t>readout_network_layer_sizes</t>
         </is>
       </c>
-      <c r="O1" s="5" t="inlineStr">
+      <c r="O1" s="7" t="inlineStr">
         <is>
           <t>readout_network_nonlinearities</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="P1" s="7" t="inlineStr">
         <is>
           <t>readout_network_dropouts</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="4">
-      <c r="A2" s="6" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2025-09-09 11:08:49</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>0000-00-00/a/0000</t>
         </is>
       </c>
-      <c r="E2" s="6" t="inlineStr">
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="F2" s="6" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>['embedding_dim___', 10]</t>
         </is>
       </c>
-      <c r="G2" s="6" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I2" s="6" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.RNN</t>
         </is>
       </c>
-      <c r="J2" s="6" t="n">
+      <c r="J2" t="n">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="n">
+      <c r="K2" t="n">
         <v>20</v>
       </c>
-      <c r="L2" s="6" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>tanh</t>
         </is>
       </c>
-      <c r="M2" s="6" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N2" s="6" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>[20, 20, 2]</t>
         </is>
       </c>
-      <c r="O2" s="6" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P2" s="6" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="4">
-      <c r="A3" s="6" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2025-09-09 11:09:25</t>
         </is>
       </c>
-      <c r="B3" s="6" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C3" s="6" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>0000-00-00/b/0000</t>
         </is>
       </c>
-      <c r="E3" s="6" t="inlineStr">
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="F3" s="6" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>['embedding_dim___', 10]</t>
         </is>
       </c>
-      <c r="G3" s="6" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H3" s="6" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I3" s="6" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.GRU</t>
         </is>
       </c>
-      <c r="J3" s="6" t="n">
+      <c r="J3" t="n">
         <v>10</v>
       </c>
-      <c r="K3" s="6" t="n">
+      <c r="K3" t="n">
         <v>20</v>
       </c>
-      <c r="M3" s="6" t="inlineStr">
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N3" s="6" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>[20, 20, 2]</t>
         </is>
       </c>
-      <c r="O3" s="6" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P3" s="6" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="4">
-      <c r="A4" s="6" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2025-09-09 11:12:01</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>2025-09-09/b/0000</t>
         </is>
       </c>
-      <c r="E4" s="6" t="inlineStr">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="G4" s="6" t="inlineStr">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H4" s="6" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I4" s="6" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.GRU</t>
         </is>
       </c>
-      <c r="J4" s="6" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>embedding_dim___</t>
         </is>
       </c>
-      <c r="K4" s="6" t="n">
+      <c r="K4" t="n">
         <v>20</v>
       </c>
-      <c r="M4" s="6" t="inlineStr">
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N4" s="6" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>[20, 20, 2]</t>
         </is>
       </c>
-      <c r="O4" s="6" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P4" s="6" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" s="4">
-      <c r="A5" s="6" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2025-09-09 11:12:27</t>
         </is>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>2025-09-09/a/0000</t>
         </is>
       </c>
-      <c r="E5" s="6" t="inlineStr">
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="G5" s="6" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H5" s="6" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I5" s="6" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.RNN</t>
         </is>
       </c>
-      <c r="J5" s="6" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>embedding_dim___</t>
         </is>
       </c>
-      <c r="K5" s="6" t="n">
+      <c r="K5" t="n">
         <v>20</v>
       </c>
-      <c r="L5" s="6" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>tanh</t>
         </is>
       </c>
-      <c r="M5" s="6" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N5" s="6" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>[20, 20, 2]</t>
         </is>
       </c>
-      <c r="O5" s="6" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P5" s="6" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" s="4">
-      <c r="A6" s="6" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2025-09-09 11:12:44</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>2025-09-09/a/0001</t>
         </is>
       </c>
-      <c r="E6" s="6" t="inlineStr">
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="G6" s="6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H6" s="6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I6" s="6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.RNN</t>
         </is>
       </c>
-      <c r="J6" s="6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>embedding_dim___</t>
         </is>
       </c>
-      <c r="K6" s="6" t="n">
+      <c r="K6" t="n">
         <v>100</v>
       </c>
-      <c r="L6" s="6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>tanh</t>
         </is>
       </c>
-      <c r="M6" s="6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N6" s="6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>[100, 20, 2]</t>
         </is>
       </c>
-      <c r="O6" s="6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P6" s="6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" s="4">
-      <c r="A7" s="6" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>2025-09-09 11:13:04</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C7" s="6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>2025-09-09/a/0002</t>
         </is>
       </c>
-      <c r="E7" s="6" t="inlineStr">
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="G7" s="6" t="inlineStr">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H7" s="6" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I7" s="6" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.RNN</t>
         </is>
       </c>
-      <c r="J7" s="6" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>embedding_dim___</t>
         </is>
       </c>
-      <c r="K7" s="6" t="n">
+      <c r="K7" t="n">
         <v>1000</v>
       </c>
-      <c r="L7" s="6" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>tanh</t>
         </is>
       </c>
-      <c r="M7" s="6" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N7" s="6" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>[1000, 20, 2]</t>
         </is>
       </c>
-      <c r="O7" s="6" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P7" s="6" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-10-14 18:07:57</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>models</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-10-14/b/0000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>models.networks.FCN</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[None]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>torch.nn.modules.rnn.GRU</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>embedding_dim___</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>20</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>models.networks.FCN</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>[20, 2]</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>[CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>[None]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1339,1452 +1414,1452 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:18</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0000</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr"/>
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>[1.0, 1e-08]</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>128</v>
-      </c>
-      <c r="J2" t="n">
-        <v>128</v>
-      </c>
-      <c r="K2" t="inlineStr">
+      <c r="I2" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K2" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L2" t="n">
+      <c r="L2" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:21</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0001</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr"/>
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>[1.0, 3.162277660168379e-08]</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>128</v>
-      </c>
-      <c r="J3" t="n">
-        <v>128</v>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="I3" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K3" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L3" t="n">
+      <c r="L3" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:23</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0002</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr"/>
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>[1.0, 1e-07]</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>128</v>
-      </c>
-      <c r="J4" t="n">
-        <v>128</v>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="I4" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K4" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L4" t="n">
+      <c r="L4" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N4" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:25</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0003</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr"/>
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>[1.0, 3.162277660168379e-07]</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I5" t="n">
-        <v>128</v>
-      </c>
-      <c r="J5" t="n">
-        <v>128</v>
-      </c>
-      <c r="K5" t="inlineStr">
+      <c r="I5" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K5" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L5" t="n">
+      <c r="L5" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N5" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:27</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0004</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
+      <c r="D6" s="6" t="inlineStr"/>
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="6" t="inlineStr">
         <is>
           <t>[1.0, 1e-06]</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I6" t="n">
-        <v>128</v>
-      </c>
-      <c r="J6" t="n">
-        <v>128</v>
-      </c>
-      <c r="K6" t="inlineStr">
+      <c r="I6" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K6" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L6" t="n">
+      <c r="L6" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N6" t="n">
+      <c r="N6" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:30</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0005</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr"/>
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>[1.0, 3.162277660168379e-06]</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I7" t="n">
-        <v>128</v>
-      </c>
-      <c r="J7" t="n">
-        <v>128</v>
-      </c>
-      <c r="K7" t="inlineStr">
+      <c r="I7" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K7" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L7" t="n">
+      <c r="L7" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M7" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N7" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:32</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0006</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
+      <c r="D8" s="6" t="inlineStr"/>
+      <c r="E8" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="6" t="inlineStr">
         <is>
           <t>[1.0, 1e-05]</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I8" t="n">
-        <v>128</v>
-      </c>
-      <c r="J8" t="n">
-        <v>128</v>
-      </c>
-      <c r="K8" t="inlineStr">
+      <c r="I8" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K8" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L8" t="n">
+      <c r="L8" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M8" t="n">
+      <c r="M8" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N8" t="n">
+      <c r="N8" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:34</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0007</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
+      <c r="D9" s="6" t="inlineStr"/>
+      <c r="E9" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="6" t="inlineStr">
         <is>
           <t>[1.0, 3.1622776601683795e-05]</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I9" t="n">
-        <v>128</v>
-      </c>
-      <c r="J9" t="n">
-        <v>128</v>
-      </c>
-      <c r="K9" t="inlineStr">
+      <c r="I9" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K9" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L9" t="n">
+      <c r="L9" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M9" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N9" t="n">
+      <c r="N9" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:37</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0008</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr"/>
+      <c r="E10" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.0001]</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G10" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H10" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I10" t="n">
-        <v>128</v>
-      </c>
-      <c r="J10" t="n">
-        <v>128</v>
-      </c>
-      <c r="K10" t="inlineStr">
+      <c r="I10" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K10" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L10" t="n">
+      <c r="L10" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M10" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N10" t="n">
+      <c r="N10" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:39</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0009</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
+      <c r="D11" s="6" t="inlineStr"/>
+      <c r="E11" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.00031622776601683794]</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H11" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I11" t="n">
-        <v>128</v>
-      </c>
-      <c r="J11" t="n">
-        <v>128</v>
-      </c>
-      <c r="K11" t="inlineStr">
+      <c r="I11" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J11" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K11" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L11" t="n">
+      <c r="L11" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M11" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N11" t="n">
+      <c r="N11" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:41</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0010</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
+      <c r="D12" s="6" t="inlineStr"/>
+      <c r="E12" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.001]</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H12" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I12" t="n">
-        <v>128</v>
-      </c>
-      <c r="J12" t="n">
-        <v>128</v>
-      </c>
-      <c r="K12" t="inlineStr">
+      <c r="I12" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J12" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K12" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L12" t="n">
+      <c r="L12" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M12" t="n">
+      <c r="M12" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N12" t="n">
+      <c r="N12" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:43</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0011</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
+      <c r="D13" s="6" t="inlineStr"/>
+      <c r="E13" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.0031622776601683794]</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="H13" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I13" t="n">
-        <v>128</v>
-      </c>
-      <c r="J13" t="n">
-        <v>128</v>
-      </c>
-      <c r="K13" t="inlineStr">
+      <c r="I13" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J13" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K13" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L13" t="n">
+      <c r="L13" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M13" t="n">
+      <c r="M13" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N13" t="n">
+      <c r="N13" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:46</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0012</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr"/>
+      <c r="E14" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.01]</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H14" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I14" t="n">
-        <v>128</v>
-      </c>
-      <c r="J14" t="n">
-        <v>128</v>
-      </c>
-      <c r="K14" t="inlineStr">
+      <c r="I14" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J14" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K14" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L14" t="n">
+      <c r="L14" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M14" t="n">
+      <c r="M14" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N14" t="n">
+      <c r="N14" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:48</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0013</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
+      <c r="D15" s="6" t="inlineStr"/>
+      <c r="E15" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.03162277660168379]</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H15" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I15" t="n">
-        <v>128</v>
-      </c>
-      <c r="J15" t="n">
-        <v>128</v>
-      </c>
-      <c r="K15" t="inlineStr">
+      <c r="I15" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J15" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K15" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L15" t="n">
+      <c r="L15" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M15" t="n">
+      <c r="M15" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N15" t="n">
+      <c r="N15" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:50</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0014</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
+      <c r="D16" s="6" t="inlineStr"/>
+      <c r="E16" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.1]</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="H16" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I16" t="n">
-        <v>128</v>
-      </c>
-      <c r="J16" t="n">
-        <v>128</v>
-      </c>
-      <c r="K16" t="inlineStr">
+      <c r="I16" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J16" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K16" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L16" t="n">
+      <c r="L16" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M16" t="n">
+      <c r="M16" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N16" t="n">
+      <c r="N16" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:53</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0015</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
+      <c r="D17" s="6" t="inlineStr"/>
+      <c r="E17" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.31622776601683794]</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G17" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="H17" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I17" t="n">
-        <v>128</v>
-      </c>
-      <c r="J17" t="n">
-        <v>128</v>
-      </c>
-      <c r="K17" t="inlineStr">
+      <c r="I17" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J17" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K17" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L17" t="n">
+      <c r="L17" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M17" t="n">
+      <c r="M17" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N17" t="n">
+      <c r="N17" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 10:52:55</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/b/0016</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr">
+      <c r="D18" s="6" t="inlineStr"/>
+      <c r="E18" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" s="6" t="inlineStr">
         <is>
           <t>[1.0, 1.0]</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="H18" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I18" t="n">
-        <v>128</v>
-      </c>
-      <c r="J18" t="n">
-        <v>128</v>
-      </c>
-      <c r="K18" t="inlineStr">
+      <c r="I18" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J18" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K18" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L18" t="n">
+      <c r="L18" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M18" t="n">
+      <c r="M18" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N18" t="n">
+      <c r="N18" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 11:27:30</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="6" t="inlineStr">
         <is>
           <t>configs/training/0000-00-00/b/0000</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr">
+      <c r="D19" s="6" t="inlineStr"/>
+      <c r="E19" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" s="6" t="inlineStr">
         <is>
           <t>[1.0, 1.0]</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="H19" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I19" t="n">
-        <v>128</v>
-      </c>
-      <c r="J19" t="n">
-        <v>128</v>
-      </c>
-      <c r="K19" t="inlineStr">
+      <c r="I19" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J19" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K19" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L19" t="n">
+      <c r="L19" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M19" t="n">
+      <c r="M19" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N19" t="n">
+      <c r="N19" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 11:36:59</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="6" t="inlineStr">
         <is>
           <t>configs/training/0000-00-00/a/0000</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
+      <c r="D20" s="6" t="inlineStr"/>
+      <c r="E20" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy']</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" s="6" t="inlineStr">
         <is>
           <t>[1.0]</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="H20" s="6" t="inlineStr">
         <is>
           <t>[0.001]</t>
         </is>
       </c>
-      <c r="I20" t="n">
-        <v>128</v>
-      </c>
-      <c r="J20" t="n">
-        <v>128</v>
-      </c>
-      <c r="K20" t="inlineStr">
+      <c r="I20" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J20" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K20" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L20" t="n">
+      <c r="L20" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M20" t="n">
+      <c r="M20" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N20" t="n">
+      <c r="N20" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 15:27:52</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/a/0001</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
+      <c r="D21" s="6" t="inlineStr"/>
+      <c r="E21" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy']</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" s="6" t="inlineStr">
         <is>
           <t>[1.0]</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G21" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adamw.AdamW']</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="H21" s="6" t="inlineStr">
         <is>
           <t>[0.001]</t>
         </is>
       </c>
-      <c r="I21" t="n">
-        <v>128</v>
-      </c>
-      <c r="J21" t="n">
-        <v>128</v>
-      </c>
-      <c r="K21" t="inlineStr">
+      <c r="I21" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J21" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K21" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L21" t="n">
+      <c r="L21" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M21" t="n">
+      <c r="M21" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N21" t="n">
+      <c r="N21" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 16:41:43</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-05/a/0000</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr">
+      <c r="D22" s="6" t="inlineStr"/>
+      <c r="E22" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy']</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" s="6" t="inlineStr">
         <is>
           <t>[1.0]</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="G22" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="H22" s="6" t="inlineStr">
         <is>
           <t>[0.001]</t>
         </is>
       </c>
-      <c r="I22" t="n">
-        <v>128</v>
-      </c>
-      <c r="J22" t="n">
-        <v>128</v>
-      </c>
-      <c r="K22" t="inlineStr">
+      <c r="I22" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J22" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K22" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L22" t="n">
+      <c r="L22" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M22" t="n">
+      <c r="M22" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N22" t="n">
+      <c r="N22" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="6" t="inlineStr">
         <is>
           <t>2025-09-16 13:16:26</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-16/y/0000</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr">
+      <c r="D23" s="6" t="inlineStr"/>
+      <c r="E23" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" s="6" t="inlineStr">
         <is>
           <t>[1.0, 1.0]</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G23" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="H23" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I23" t="n">
-        <v>128</v>
-      </c>
-      <c r="J23" t="n">
-        <v>128</v>
-      </c>
-      <c r="K23" t="inlineStr">
+      <c r="I23" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J23" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K23" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L23" t="n">
+      <c r="L23" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M23" t="n">
+      <c r="M23" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N23" t="n">
+      <c r="N23" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="6" t="inlineStr">
         <is>
           <t>2025-09-16 13:29:08</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-16/z/0000</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
+      <c r="D24" s="6" t="inlineStr"/>
+      <c r="E24" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy']</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" s="6" t="inlineStr">
         <is>
           <t>[1.0]</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G24" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="H24" s="6" t="inlineStr">
         <is>
           <t>[0.001]</t>
         </is>
       </c>
-      <c r="I24" t="n">
-        <v>128</v>
-      </c>
-      <c r="J24" t="n">
-        <v>128</v>
-      </c>
-      <c r="K24" t="inlineStr">
+      <c r="I24" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J24" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K24" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L24" t="n">
+      <c r="L24" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M24" t="n">
+      <c r="M24" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N24" t="n">
+      <c r="N24" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="6" t="inlineStr">
         <is>
           <t>2025-09-16 14:13:04</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-16/x/0000</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
+      <c r="D25" s="6" t="inlineStr"/>
+      <c r="E25" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.01]</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adamw.AdamW', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="H25" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I25" t="n">
-        <v>128</v>
-      </c>
-      <c r="J25" t="n">
-        <v>128</v>
-      </c>
-      <c r="K25" t="inlineStr">
+      <c r="I25" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J25" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K25" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L25" t="n">
+      <c r="L25" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="M25" t="n">
+      <c r="M25" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N25" t="n">
+      <c r="N25" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="6" t="inlineStr">
         <is>
           <t>2025-09-16 14:27:00</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="6" t="inlineStr">
         <is>
           <t>training</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="6" t="inlineStr">
         <is>
           <t>configs/training/2025-09-16/x/0001</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr">
+      <c r="D26" s="6" t="inlineStr"/>
+      <c r="E26" s="6" t="inlineStr">
         <is>
           <t>['cross_entropy', 'spectral_entropy']</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F26" s="6" t="inlineStr">
         <is>
           <t>[1.0, 0.01]</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="G26" s="6" t="inlineStr">
         <is>
           <t>['torch.optim.adamw.AdamW', 'torch.optim.adam.Adam']</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="H26" s="6" t="inlineStr">
         <is>
           <t>[0.001, 0.001]</t>
         </is>
       </c>
-      <c r="I26" t="n">
-        <v>128</v>
-      </c>
-      <c r="J26" t="n">
-        <v>128</v>
-      </c>
-      <c r="K26" t="inlineStr">
+      <c r="I26" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="J26" s="6" t="n">
+        <v>128</v>
+      </c>
+      <c r="K26" s="6" t="inlineStr">
         <is>
           <t>general_utils.ml.training.NoImprovementStopping</t>
         </is>
       </c>
-      <c r="L26" t="n">
+      <c r="L26" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="M26" t="n">
+      <c r="M26" s="6" t="n">
         <v>1e-05</v>
       </c>
-      <c r="N26" t="n">
+      <c r="N26" s="6" t="n">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prepare for experiments/2025-11-18/0000. Also update README for configs/training/2025-09-16/y and remove README for configs/training/2025-09-16/x which was clearly incorrect and informative.
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -461,392 +461,392 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>2025-09-04 16:09:19</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>0000-00-00/a/0000</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
+      <c r="D2" s="6" t="inlineStr"/>
+      <c r="E2" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>[[1, 0], [1, 1]]</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="6" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="6" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4]</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="6" t="inlineStr">
         <is>
           <t>[0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224]</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="6" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4]</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" s="6" t="inlineStr">
         <is>
           <t>[0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224]</t>
         </is>
       </c>
-      <c r="M2" t="n">
+      <c r="M2" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2" s="6" t="n">
         <v>500</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2" s="6" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 11:06:37</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>2025-09-05/a/0000</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
+      <c r="D3" s="6" t="inlineStr"/>
+      <c r="E3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>[[1, 0], [1, 1]]</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="6" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="6" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="6" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19]</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="6" t="inlineStr">
         <is>
           <t>[0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806, 0.05000000074505806]</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" s="6" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9]</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L3" s="6" t="inlineStr">
         <is>
           <t>[0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612]</t>
         </is>
       </c>
-      <c r="M3" t="n">
+      <c r="M3" s="6" t="n">
         <v>5000</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3" s="6" t="n">
         <v>2500</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O3" s="6" t="n">
         <v>2500</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 14:00:39</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>2025-09-05/o/0000</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
+      <c r="D4" s="6" t="inlineStr"/>
+      <c r="E4" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>[[1, 0], [1, 1]]</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="6" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="6" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" s="6" t="inlineStr">
         <is>
           <t>[1, 3, 5, 7, 9, 11, 13, 15, 17, 19]</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="6" t="inlineStr">
         <is>
           <t>[0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612]</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K4" s="6" t="inlineStr">
         <is>
           <t>[1, 3, 5, 7, 9]</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L4" s="6" t="inlineStr">
         <is>
           <t>[0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224]</t>
         </is>
       </c>
-      <c r="M4" t="n">
+      <c r="M4" s="6" t="n">
         <v>5000</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N4" s="6" t="n">
         <v>2500</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O4" s="6" t="n">
         <v>2500</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>2025-09-05 14:01:02</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>2025-09-05/e/0000</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="n">
+      <c r="D5" s="6" t="inlineStr"/>
+      <c r="E5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>[[1, 0], [1, 1]]</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="6" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="6" t="inlineStr">
         <is>
           <t>[0.5, 0.5]</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="6" t="inlineStr">
         <is>
           <t>[0, 2, 4, 6, 8, 10, 12, 14, 16, 18, 20]</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" s="6" t="inlineStr">
         <is>
           <t>[0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294]</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="K5" s="6" t="inlineStr">
         <is>
           <t>[0, 2, 4, 6, 8, 10]</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L5" s="6" t="inlineStr">
         <is>
           <t>[0.1666666716337204, 0.1666666716337204, 0.1666666716337204, 0.1666666716337204, 0.1666666716337204, 0.1666666716337204]</t>
         </is>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" s="6" t="n">
         <v>5000</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N5" s="6" t="n">
         <v>2500</v>
       </c>
-      <c r="O5" t="n">
+      <c r="O5" s="6" t="n">
         <v>2500</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>2025-10-23 16:38:36</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>2025-10-23/e/0000</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="n">
+      <c r="D6" s="6" t="inlineStr"/>
+      <c r="E6" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="6" t="inlineStr">
         <is>
           <t>[[0, 1, 0], [0, 1, 1], [1, 0, 1], [1, 1, 1]]</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" s="6" t="inlineStr">
         <is>
           <t>[0.25, 0.25, 0.25, 0.25]</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="6" t="inlineStr">
         <is>
           <t>[0.25, 0.25, 0.25, 0.25]</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" s="6" t="inlineStr">
         <is>
           <t>[0, 2, 4, 6, 8, 10, 12, 14, 16, 18, 20]</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="J6" s="6" t="inlineStr">
         <is>
           <t>[0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294, 0.09090909361839294]</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="K6" s="6" t="inlineStr">
         <is>
           <t>[0, 2, 4, 6, 8, 10]</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="L6" s="6" t="inlineStr">
         <is>
           <t>[0.1666666716337204, 0.1666666716337204, 0.1666666716337204, 0.1666666716337204, 0.1666666716337204, 0.1666666716337204]</t>
         </is>
       </c>
-      <c r="M6" t="n">
+      <c r="M6" s="6" t="n">
         <v>5000</v>
       </c>
-      <c r="N6" t="n">
+      <c r="N6" s="6" t="n">
         <v>2500</v>
       </c>
-      <c r="O6" t="n">
+      <c r="O6" s="6" t="n">
         <v>2500</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>2025-10-23 16:47:03</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>datasets</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>2025-10-23/o/0000</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
+      <c r="D7" s="6" t="inlineStr"/>
+      <c r="E7" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>[[0, 1, 0], [0, 1, 1], [1, 0, 1], [1, 1, 1]]</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="6" t="inlineStr">
         <is>
           <t>[0.25, 0.25, 0.25, 0.25]</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="6" t="inlineStr">
         <is>
           <t>[0.25, 0.25, 0.25, 0.25]</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" s="6" t="inlineStr">
         <is>
           <t>[1, 3, 5, 7, 9, 11, 13, 15, 17, 19]</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J7" s="6" t="inlineStr">
         <is>
           <t>[0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612, 0.10000000149011612]</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K7" s="6" t="inlineStr">
         <is>
           <t>[1, 3, 5, 7, 9]</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L7" s="6" t="inlineStr">
         <is>
           <t>[0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224, 0.20000000298023224]</t>
         </is>
       </c>
-      <c r="M7" t="n">
+      <c r="M7" s="6" t="n">
         <v>5000</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N7" s="6" t="n">
         <v>2500</v>
       </c>
-      <c r="O7" t="n">
+      <c r="O7" s="6" t="n">
         <v>2500</v>
       </c>
     </row>
@@ -857,585 +857,670 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>timestamp</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>config_kind</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>config_id</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>input_network</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>input_network_layer_sizes</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>input_network_nonlinearities</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>input_network_dropouts</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>rnn_type</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>rnn_input_size</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>rnn_hidden_size</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>rnn_nonlinearity</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>readout_network</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>readout_network_layer_sizes</t>
         </is>
       </c>
-      <c r="O1" s="5" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>readout_network_nonlinearities</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>readout_network_dropouts</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="4">
-      <c r="A2" s="6" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2025-09-09 11:08:49</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>0000-00-00/a/0000</t>
         </is>
       </c>
-      <c r="E2" s="6" t="inlineStr">
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="F2" s="6" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>['embedding_dim___', 10]</t>
         </is>
       </c>
-      <c r="G2" s="6" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I2" s="6" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.RNN</t>
         </is>
       </c>
-      <c r="J2" s="6" t="n">
+      <c r="J2" t="n">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="n">
+      <c r="K2" t="n">
         <v>20</v>
       </c>
-      <c r="L2" s="6" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>tanh</t>
         </is>
       </c>
-      <c r="M2" s="6" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N2" s="6" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>[20, 20, 2]</t>
         </is>
       </c>
-      <c r="O2" s="6" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P2" s="6" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="4">
-      <c r="A3" s="6" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2025-09-09 11:09:25</t>
         </is>
       </c>
-      <c r="B3" s="6" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C3" s="6" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>0000-00-00/b/0000</t>
         </is>
       </c>
-      <c r="E3" s="6" t="inlineStr">
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="F3" s="6" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>['embedding_dim___', 10]</t>
         </is>
       </c>
-      <c r="G3" s="6" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H3" s="6" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I3" s="6" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.GRU</t>
         </is>
       </c>
-      <c r="J3" s="6" t="n">
+      <c r="J3" t="n">
         <v>10</v>
       </c>
-      <c r="K3" s="6" t="n">
+      <c r="K3" t="n">
         <v>20</v>
       </c>
-      <c r="M3" s="6" t="inlineStr">
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N3" s="6" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>[20, 20, 2]</t>
         </is>
       </c>
-      <c r="O3" s="6" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P3" s="6" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="4">
-      <c r="A4" s="6" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2025-09-09 11:12:01</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>2025-09-09/b/0000</t>
         </is>
       </c>
-      <c r="E4" s="6" t="inlineStr">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="G4" s="6" t="inlineStr">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H4" s="6" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I4" s="6" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.GRU</t>
         </is>
       </c>
-      <c r="J4" s="6" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>embedding_dim___</t>
         </is>
       </c>
-      <c r="K4" s="6" t="n">
+      <c r="K4" t="n">
         <v>20</v>
       </c>
-      <c r="M4" s="6" t="inlineStr">
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N4" s="6" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>[20, 20, 2]</t>
         </is>
       </c>
-      <c r="O4" s="6" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P4" s="6" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" s="4">
-      <c r="A5" s="6" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2025-09-09 11:12:27</t>
         </is>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>2025-09-09/a/0000</t>
         </is>
       </c>
-      <c r="E5" s="6" t="inlineStr">
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="G5" s="6" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H5" s="6" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I5" s="6" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.RNN</t>
         </is>
       </c>
-      <c r="J5" s="6" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>embedding_dim___</t>
         </is>
       </c>
-      <c r="K5" s="6" t="n">
+      <c r="K5" t="n">
         <v>20</v>
       </c>
-      <c r="L5" s="6" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>tanh</t>
         </is>
       </c>
-      <c r="M5" s="6" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N5" s="6" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>[20, 20, 2]</t>
         </is>
       </c>
-      <c r="O5" s="6" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P5" s="6" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" s="4">
-      <c r="A6" s="6" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2025-09-09 11:12:44</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>2025-09-09/a/0001</t>
         </is>
       </c>
-      <c r="E6" s="6" t="inlineStr">
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="G6" s="6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H6" s="6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I6" s="6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.RNN</t>
         </is>
       </c>
-      <c r="J6" s="6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>embedding_dim___</t>
         </is>
       </c>
-      <c r="K6" s="6" t="n">
+      <c r="K6" t="n">
         <v>100</v>
       </c>
-      <c r="L6" s="6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>tanh</t>
         </is>
       </c>
-      <c r="M6" s="6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N6" s="6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>[100, 20, 2]</t>
         </is>
       </c>
-      <c r="O6" s="6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P6" s="6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" s="4">
-      <c r="A7" s="6" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>2025-09-09 11:13:04</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C7" s="6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>2025-09-09/a/0002</t>
         </is>
       </c>
-      <c r="E7" s="6" t="inlineStr">
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="G7" s="6" t="inlineStr">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H7" s="6" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I7" s="6" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.RNN</t>
         </is>
       </c>
-      <c r="J7" s="6" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>embedding_dim___</t>
         </is>
       </c>
-      <c r="K7" s="6" t="n">
+      <c r="K7" t="n">
         <v>1000</v>
       </c>
-      <c r="L7" s="6" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>tanh</t>
         </is>
       </c>
-      <c r="M7" s="6" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N7" s="6" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>[1000, 20, 2]</t>
         </is>
       </c>
-      <c r="O7" s="6" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.GELU', args_cfg=GELUConfig(approximate='none'), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print'), CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P7" s="6" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>[0.5, None]</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="4">
-      <c r="A8" s="6" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>2025-10-14 18:07:57</t>
         </is>
       </c>
-      <c r="B8" s="6" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>models</t>
         </is>
       </c>
-      <c r="C8" s="6" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>2025-10-14/b/0000</t>
         </is>
       </c>
-      <c r="E8" s="6" t="inlineStr">
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="G8" s="6" t="inlineStr">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="H8" s="6" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
-      <c r="I8" s="6" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>torch.nn.modules.rnn.GRU</t>
         </is>
       </c>
-      <c r="J8" s="6" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>embedding_dim___</t>
         </is>
       </c>
-      <c r="K8" s="6" t="n">
+      <c r="K8" t="n">
         <v>20</v>
       </c>
-      <c r="M8" s="6" t="inlineStr">
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
         <is>
           <t>models.networks.FCN</t>
         </is>
       </c>
-      <c r="N8" s="6" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>[20, 2]</t>
         </is>
       </c>
-      <c r="O8" s="6" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>[CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
         </is>
       </c>
-      <c r="P8" s="6" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-11-18 15:24:17</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>models</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-11-18/a/0000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>models.networks.FCN</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[None]</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>torch.nn.modules.rnn.RNN</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>embedding_dim___</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>20</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>models.networks.FCN</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>[20, 2]</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>[CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>[None]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Prepare for call to experiments/2025-11-18/0001/run.py.
</commit_message>
<xml_diff>
--- a/configs/logs.xlsx
+++ b/configs/logs.xlsx
@@ -861,7 +861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1514,6 +1514,78 @@
         </is>
       </c>
       <c r="P9" t="inlineStr">
+        <is>
+          <t>[None]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-11-18 15:48:05</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>models</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-11-18/a/0001</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>models.networks.FCN</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>[CallableConfig(path='torch.nn.modules.activation.ReLU', args_cfg=ReLUConfig(inplace=False), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[None]</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>torch.nn.modules.rnn.RNN</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>embedding_dim___</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>20</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>models.networks.FCN</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>[20, 2]</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>[CallableConfig(path='torch.nn.modules.linear.Identity', args_cfg=IdentityConfig(), kind='class', recovery_mode='call', locked=False, if_recover_while_locked='print')]</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
         <is>
           <t>[None]</t>
         </is>

</xml_diff>